<commit_message>
update some bullshit code
</commit_message>
<xml_diff>
--- a/data/Survey.xlsx
+++ b/data/Survey.xlsx
@@ -876,13 +876,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -994,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1008,12 +1008,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1023,34 +1017,31 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1458,93 +1449,93 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -1579,1392 +1570,1392 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="9">
         <v>24</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="14">
+      <c r="T2" s="11">
         <v>2</v>
       </c>
-      <c r="U2" s="14">
+      <c r="U2" s="11">
         <v>3</v>
       </c>
-      <c r="V2" s="14">
-        <v>6</v>
-      </c>
-      <c r="W2" s="14">
+      <c r="V2" s="11">
+        <v>6</v>
+      </c>
+      <c r="W2" s="11">
         <v>2</v>
       </c>
-      <c r="X2" s="14">
-        <v>6</v>
-      </c>
-      <c r="Y2" s="14">
-        <v>6</v>
-      </c>
-      <c r="Z2" s="14">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="14">
+      <c r="X2" s="11">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="11">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="11">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="11">
         <v>2</v>
       </c>
-      <c r="AB2" s="14">
-        <v>6</v>
-      </c>
-      <c r="AC2" s="14">
+      <c r="AB2" s="11">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="11">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="12">
+      <c r="O3" s="10"/>
+      <c r="P3" s="9">
         <v>23</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="15">
-        <v>5</v>
-      </c>
-      <c r="U3" s="15">
-        <v>5</v>
-      </c>
-      <c r="V3" s="15">
-        <v>4</v>
-      </c>
-      <c r="W3" s="15">
-        <v>4</v>
-      </c>
-      <c r="X3" s="15">
+      <c r="T3" s="12">
+        <v>5</v>
+      </c>
+      <c r="U3" s="12">
+        <v>5</v>
+      </c>
+      <c r="V3" s="12">
+        <v>4</v>
+      </c>
+      <c r="W3" s="12">
+        <v>4</v>
+      </c>
+      <c r="X3" s="12">
         <v>3</v>
       </c>
-      <c r="Y3" s="15">
+      <c r="Y3" s="12">
         <v>3</v>
       </c>
-      <c r="Z3" s="15">
-        <v>6</v>
-      </c>
-      <c r="AA3" s="15">
+      <c r="Z3" s="12">
+        <v>6</v>
+      </c>
+      <c r="AA3" s="12">
         <v>2</v>
       </c>
-      <c r="AB3" s="15">
-        <v>4</v>
-      </c>
-      <c r="AC3" s="15">
+      <c r="AB3" s="12">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="12">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13" t="s">
+      <c r="M4" s="10"/>
+      <c r="N4" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="12">
+      <c r="O4" s="10"/>
+      <c r="P4" s="9">
         <v>24</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="T4" s="15">
-        <v>5</v>
-      </c>
-      <c r="U4" s="15">
-        <v>4</v>
-      </c>
-      <c r="V4" s="15">
-        <v>4</v>
-      </c>
-      <c r="W4" s="15">
-        <v>4</v>
-      </c>
-      <c r="X4" s="15">
-        <v>4</v>
-      </c>
-      <c r="Y4" s="15">
-        <v>4</v>
-      </c>
-      <c r="Z4" s="15">
-        <v>4</v>
-      </c>
-      <c r="AA4" s="15">
+      <c r="T4" s="12">
+        <v>5</v>
+      </c>
+      <c r="U4" s="12">
+        <v>4</v>
+      </c>
+      <c r="V4" s="12">
+        <v>4</v>
+      </c>
+      <c r="W4" s="12">
+        <v>4</v>
+      </c>
+      <c r="X4" s="12">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="12">
         <v>3</v>
       </c>
-      <c r="AB4" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC4" s="15">
+      <c r="AB4" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="12">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="12">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13" t="s">
+      <c r="M5" s="10"/>
+      <c r="N5" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="9">
         <v>24</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="Q5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="T5" s="15">
+      <c r="T5" s="12">
         <v>2</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U5" s="12">
         <v>2</v>
       </c>
-      <c r="V5" s="15">
-        <v>4</v>
-      </c>
-      <c r="W5" s="15">
-        <v>5</v>
-      </c>
-      <c r="X5" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y5" s="15">
+      <c r="V5" s="12">
+        <v>4</v>
+      </c>
+      <c r="W5" s="12">
+        <v>5</v>
+      </c>
+      <c r="X5" s="12">
+        <v>6</v>
+      </c>
+      <c r="Y5" s="12">
         <v>3</v>
       </c>
-      <c r="Z5" s="15">
+      <c r="Z5" s="12">
         <v>7</v>
       </c>
-      <c r="AA5" s="15">
+      <c r="AA5" s="12">
         <v>2</v>
       </c>
-      <c r="AB5" s="15">
-        <v>6</v>
-      </c>
-      <c r="AC5" s="15">
+      <c r="AB5" s="12">
+        <v>6</v>
+      </c>
+      <c r="AC5" s="12">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="12">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13" t="s">
+      <c r="M6" s="10"/>
+      <c r="N6" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="9">
         <v>28</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="Q6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="S6" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="15">
+      <c r="T6" s="12">
         <v>3</v>
       </c>
-      <c r="U6" s="15">
+      <c r="U6" s="12">
         <v>3</v>
       </c>
-      <c r="V6" s="15">
-        <v>5</v>
-      </c>
-      <c r="W6" s="15">
+      <c r="V6" s="12">
+        <v>5</v>
+      </c>
+      <c r="W6" s="12">
         <v>3</v>
       </c>
-      <c r="X6" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y6" s="15">
+      <c r="X6" s="12">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="12">
         <v>3</v>
       </c>
-      <c r="Z6" s="15">
-        <v>6</v>
-      </c>
-      <c r="AA6" s="15">
+      <c r="Z6" s="12">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="12">
         <v>3</v>
       </c>
-      <c r="AB6" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC6" s="15">
+      <c r="AB6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="12">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="12">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13" t="s">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13" t="s">
+      <c r="M7" s="10"/>
+      <c r="N7" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="9">
         <v>23</v>
       </c>
-      <c r="Q7" s="13" t="s">
+      <c r="Q7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="T7" s="15">
+      <c r="T7" s="12">
         <v>7</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="12">
         <v>1</v>
       </c>
-      <c r="V7" s="15">
-        <v>6</v>
-      </c>
-      <c r="W7" s="15">
-        <v>4</v>
-      </c>
-      <c r="X7" s="15">
+      <c r="V7" s="12">
+        <v>6</v>
+      </c>
+      <c r="W7" s="12">
+        <v>4</v>
+      </c>
+      <c r="X7" s="12">
         <v>7</v>
       </c>
-      <c r="Y7" s="15">
-        <v>5</v>
-      </c>
-      <c r="Z7" s="15">
-        <v>6</v>
-      </c>
-      <c r="AA7" s="15">
+      <c r="Y7" s="12">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="12">
         <v>3</v>
       </c>
-      <c r="AB7" s="15">
-        <v>6</v>
-      </c>
-      <c r="AC7" s="15">
+      <c r="AB7" s="12">
+        <v>6</v>
+      </c>
+      <c r="AC7" s="12">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13" t="s">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13" t="s">
+      <c r="M8" s="10"/>
+      <c r="N8" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="9">
         <v>24</v>
       </c>
-      <c r="Q8" s="13" t="s">
+      <c r="Q8" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="S8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="T8" s="15">
-        <v>4</v>
-      </c>
-      <c r="U8" s="15">
+      <c r="T8" s="12">
+        <v>4</v>
+      </c>
+      <c r="U8" s="12">
         <v>3</v>
       </c>
-      <c r="V8" s="15">
-        <v>5</v>
-      </c>
-      <c r="W8" s="15">
+      <c r="V8" s="12">
+        <v>5</v>
+      </c>
+      <c r="W8" s="12">
         <v>2</v>
       </c>
-      <c r="X8" s="15">
-        <v>4</v>
-      </c>
-      <c r="Y8" s="15">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="15">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="15">
+      <c r="X8" s="12">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="12">
         <v>3</v>
       </c>
-      <c r="AB8" s="15">
-        <v>6</v>
-      </c>
-      <c r="AC8" s="15">
+      <c r="AB8" s="12">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="12">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="12">
+      <c r="O9" s="10"/>
+      <c r="P9" s="9">
         <v>24</v>
       </c>
-      <c r="Q9" s="13" t="s">
+      <c r="Q9" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R9" s="13" t="s">
+      <c r="R9" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="S9" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="T9" s="15">
-        <v>4</v>
-      </c>
-      <c r="U9" s="15">
+      <c r="T9" s="12">
+        <v>4</v>
+      </c>
+      <c r="U9" s="12">
         <v>3</v>
       </c>
-      <c r="V9" s="15">
-        <v>5</v>
-      </c>
-      <c r="W9" s="15">
-        <v>4</v>
-      </c>
-      <c r="X9" s="15">
-        <v>5</v>
-      </c>
-      <c r="Y9" s="15">
-        <v>6</v>
-      </c>
-      <c r="Z9" s="15">
-        <v>4</v>
-      </c>
-      <c r="AA9" s="15">
+      <c r="V9" s="12">
+        <v>5</v>
+      </c>
+      <c r="W9" s="12">
+        <v>4</v>
+      </c>
+      <c r="X9" s="12">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="12">
         <v>3</v>
       </c>
-      <c r="AB9" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC9" s="15">
+      <c r="AB9" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="12">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
+      <c r="I10" s="10"/>
+      <c r="J10" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13" t="s">
+      <c r="M10" s="10"/>
+      <c r="N10" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="O10" s="13"/>
-      <c r="P10" s="12">
+      <c r="O10" s="10"/>
+      <c r="P10" s="9">
         <v>27</v>
       </c>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="13" t="s">
+      <c r="R10" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="S10" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="T10" s="15">
+      <c r="T10" s="12">
         <v>3</v>
       </c>
-      <c r="U10" s="15">
+      <c r="U10" s="12">
         <v>2</v>
       </c>
-      <c r="V10" s="15">
-        <v>6</v>
-      </c>
-      <c r="W10" s="15">
+      <c r="V10" s="12">
+        <v>6</v>
+      </c>
+      <c r="W10" s="12">
         <v>3</v>
       </c>
-      <c r="X10" s="15">
-        <v>4</v>
-      </c>
-      <c r="Y10" s="15">
-        <v>5</v>
-      </c>
-      <c r="Z10" s="15">
-        <v>5</v>
-      </c>
-      <c r="AA10" s="15">
+      <c r="X10" s="12">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="12">
         <v>1</v>
       </c>
-      <c r="AB10" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC10" s="15">
+      <c r="AB10" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC10" s="12">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="12">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="I11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13" t="s">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="O11" s="13" t="s">
+      <c r="O11" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="9">
         <v>23</v>
       </c>
-      <c r="Q11" s="13" t="s">
+      <c r="Q11" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R11" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="S11" s="13" t="s">
+      <c r="R11" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="S11" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="T11" s="15">
+      <c r="T11" s="12">
         <v>1</v>
       </c>
-      <c r="U11" s="15">
+      <c r="U11" s="12">
         <v>7</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="12">
         <v>7</v>
       </c>
-      <c r="W11" s="15">
-        <v>6</v>
-      </c>
-      <c r="X11" s="15">
+      <c r="W11" s="12">
+        <v>6</v>
+      </c>
+      <c r="X11" s="12">
         <v>7</v>
       </c>
-      <c r="Y11" s="15">
+      <c r="Y11" s="12">
         <v>3</v>
       </c>
-      <c r="Z11" s="15">
+      <c r="Z11" s="12">
         <v>7</v>
       </c>
-      <c r="AA11" s="15">
+      <c r="AA11" s="12">
         <v>1</v>
       </c>
-      <c r="AB11" s="15">
+      <c r="AB11" s="12">
         <v>7</v>
       </c>
-      <c r="AC11" s="15">
+      <c r="AC11" s="12">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="12">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
+      <c r="I12" s="10"/>
+      <c r="J12" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13" t="s">
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13" t="s">
+      <c r="M12" s="10"/>
+      <c r="N12" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="9">
         <v>23</v>
       </c>
-      <c r="Q12" s="13" t="s">
+      <c r="Q12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="R12" s="13" t="s">
+      <c r="R12" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="S12" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="T12" s="15">
-        <v>5</v>
-      </c>
-      <c r="U12" s="15">
+      <c r="T12" s="12">
+        <v>5</v>
+      </c>
+      <c r="U12" s="12">
         <v>2</v>
       </c>
-      <c r="V12" s="15">
-        <v>6</v>
-      </c>
-      <c r="W12" s="15">
-        <v>4</v>
-      </c>
-      <c r="X12" s="15">
+      <c r="V12" s="12">
+        <v>6</v>
+      </c>
+      <c r="W12" s="12">
+        <v>4</v>
+      </c>
+      <c r="X12" s="12">
         <v>7</v>
       </c>
-      <c r="Y12" s="15">
-        <v>6</v>
-      </c>
-      <c r="Z12" s="15">
+      <c r="Y12" s="12">
+        <v>6</v>
+      </c>
+      <c r="Z12" s="12">
         <v>7</v>
       </c>
-      <c r="AA12" s="15">
+      <c r="AA12" s="12">
         <v>2</v>
       </c>
-      <c r="AB12" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="15">
+      <c r="AB12" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="12">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="12">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
+      <c r="I13" s="10"/>
+      <c r="J13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13" t="s">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13" t="s">
+      <c r="M13" s="10"/>
+      <c r="N13" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="O13" s="13"/>
-      <c r="P13" s="12">
+      <c r="O13" s="10"/>
+      <c r="P13" s="9">
         <v>25</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="R13" s="13" t="s">
+      <c r="R13" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S13" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="T13" s="15">
-        <v>5</v>
-      </c>
-      <c r="U13" s="15">
-        <v>5</v>
-      </c>
-      <c r="V13" s="15">
-        <v>6</v>
-      </c>
-      <c r="W13" s="15">
+      <c r="T13" s="12">
+        <v>5</v>
+      </c>
+      <c r="U13" s="12">
+        <v>5</v>
+      </c>
+      <c r="V13" s="12">
+        <v>6</v>
+      </c>
+      <c r="W13" s="12">
         <v>2</v>
       </c>
-      <c r="X13" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y13" s="15">
-        <v>6</v>
-      </c>
-      <c r="Z13" s="15">
-        <v>6</v>
-      </c>
-      <c r="AA13" s="15">
-        <v>6</v>
-      </c>
-      <c r="AB13" s="15">
+      <c r="X13" s="12">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>6</v>
+      </c>
+      <c r="AA13" s="12">
+        <v>6</v>
+      </c>
+      <c r="AB13" s="12">
         <v>7</v>
       </c>
-      <c r="AC13" s="15">
+      <c r="AC13" s="12">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="12">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16" t="s">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16" t="s">
+      <c r="I14" s="13"/>
+      <c r="J14" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16" t="s">
+      <c r="K14" s="13"/>
+      <c r="L14" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16" t="s">
+      <c r="M14" s="13"/>
+      <c r="N14" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="P14" s="17">
+      <c r="P14" s="14">
         <v>21</v>
       </c>
-      <c r="Q14" s="16" t="s">
+      <c r="Q14" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="R14" s="16" t="s">
+      <c r="R14" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="S14" s="16" t="s">
+      <c r="S14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="T14" s="17">
+      <c r="T14" s="14">
         <v>3</v>
       </c>
-      <c r="U14" s="17">
+      <c r="U14" s="14">
         <v>1</v>
       </c>
-      <c r="V14" s="17">
-        <v>5</v>
-      </c>
-      <c r="W14" s="17">
+      <c r="V14" s="14">
+        <v>5</v>
+      </c>
+      <c r="W14" s="14">
         <v>7</v>
       </c>
-      <c r="X14" s="17">
-        <v>4</v>
-      </c>
-      <c r="Y14" s="17">
-        <v>5</v>
-      </c>
-      <c r="Z14" s="17">
-        <v>6</v>
-      </c>
-      <c r="AA14" s="17">
+      <c r="X14" s="14">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="14">
+        <v>5</v>
+      </c>
+      <c r="Z14" s="14">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="14">
         <v>2</v>
       </c>
-      <c r="AB14" s="17">
-        <v>5</v>
-      </c>
-      <c r="AC14" s="17">
+      <c r="AB14" s="14">
+        <v>5</v>
+      </c>
+      <c r="AC14" s="14">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="12">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16" t="s">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="O15" s="16" t="s">
+      <c r="O15" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="P15" s="17">
+      <c r="P15" s="14">
         <v>21</v>
       </c>
-      <c r="Q15" s="16" t="s">
+      <c r="Q15" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="R15" s="16" t="s">
+      <c r="R15" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="S15" s="16" t="s">
+      <c r="S15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="T15" s="17">
-        <v>5</v>
-      </c>
-      <c r="U15" s="17">
+      <c r="T15" s="14">
+        <v>5</v>
+      </c>
+      <c r="U15" s="14">
         <v>3</v>
       </c>
-      <c r="V15" s="17">
+      <c r="V15" s="14">
         <v>2</v>
       </c>
-      <c r="W15" s="17">
+      <c r="W15" s="14">
         <v>3</v>
       </c>
-      <c r="X15" s="17">
-        <v>6</v>
-      </c>
-      <c r="Y15" s="17">
+      <c r="X15" s="14">
+        <v>6</v>
+      </c>
+      <c r="Y15" s="14">
         <v>2</v>
       </c>
-      <c r="Z15" s="17">
-        <v>5</v>
-      </c>
-      <c r="AA15" s="17">
-        <v>5</v>
-      </c>
-      <c r="AB15" s="17">
+      <c r="Z15" s="14">
+        <v>5</v>
+      </c>
+      <c r="AA15" s="14">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="14">
         <v>2</v>
       </c>
-      <c r="AC15" s="17">
+      <c r="AC15" s="14">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="12">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="13"/>
+      <c r="J16" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
+      <c r="K16" s="13"/>
+      <c r="L16" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16" t="s">
+      <c r="M16" s="13"/>
+      <c r="N16" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="O16" s="16" t="s">
+      <c r="O16" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="P16" s="17">
+      <c r="P16" s="14">
         <v>22</v>
       </c>
-      <c r="Q16" s="16" t="s">
+      <c r="Q16" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="16" t="s">
+      <c r="R16" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="S16" s="16" t="s">
+      <c r="S16" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="T16" s="17">
+      <c r="T16" s="14">
         <v>3</v>
       </c>
-      <c r="U16" s="17">
+      <c r="U16" s="14">
         <v>2</v>
       </c>
-      <c r="V16" s="17">
-        <v>4</v>
-      </c>
-      <c r="W16" s="17">
-        <v>5</v>
-      </c>
-      <c r="X16" s="17">
-        <v>5</v>
-      </c>
-      <c r="Y16" s="17">
-        <v>5</v>
-      </c>
-      <c r="Z16" s="17">
-        <v>5</v>
-      </c>
-      <c r="AA16" s="17">
+      <c r="V16" s="14">
+        <v>4</v>
+      </c>
+      <c r="W16" s="14">
+        <v>5</v>
+      </c>
+      <c r="X16" s="14">
+        <v>5</v>
+      </c>
+      <c r="Y16" s="14">
+        <v>5</v>
+      </c>
+      <c r="Z16" s="14">
+        <v>5</v>
+      </c>
+      <c r="AA16" s="14">
         <v>3</v>
       </c>
-      <c r="AB16" s="17">
-        <v>4</v>
-      </c>
-      <c r="AC16" s="17">
+      <c r="AB16" s="14">
+        <v>4</v>
+      </c>
+      <c r="AC16" s="14">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="12">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16" t="s">
+      <c r="E17" s="13"/>
+      <c r="F17" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16" t="s">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16" t="s">
+      <c r="I17" s="13"/>
+      <c r="J17" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16" t="s">
+      <c r="K17" s="13"/>
+      <c r="L17" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16" t="s">
+      <c r="M17" s="13"/>
+      <c r="N17" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="O17" s="16" t="s">
+      <c r="O17" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="P17" s="17">
+      <c r="P17" s="14">
         <v>22</v>
       </c>
-      <c r="Q17" s="16" t="s">
+      <c r="Q17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="R17" s="16" t="s">
+      <c r="R17" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="S17" s="16" t="s">
+      <c r="S17" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="T17" s="17">
-        <v>6</v>
-      </c>
-      <c r="U17" s="17">
+      <c r="T17" s="14">
+        <v>6</v>
+      </c>
+      <c r="U17" s="14">
         <v>2</v>
       </c>
-      <c r="V17" s="17">
-        <v>6</v>
-      </c>
-      <c r="W17" s="17">
+      <c r="V17" s="14">
+        <v>6</v>
+      </c>
+      <c r="W17" s="14">
         <v>2</v>
       </c>
-      <c r="X17" s="17">
-        <v>6</v>
-      </c>
-      <c r="Y17" s="17">
-        <v>5</v>
-      </c>
-      <c r="Z17" s="17">
-        <v>6</v>
-      </c>
-      <c r="AA17" s="17">
+      <c r="X17" s="14">
+        <v>6</v>
+      </c>
+      <c r="Y17" s="14">
+        <v>5</v>
+      </c>
+      <c r="Z17" s="14">
+        <v>6</v>
+      </c>
+      <c r="AA17" s="14">
         <v>2</v>
       </c>
-      <c r="AB17" s="17">
-        <v>6</v>
-      </c>
-      <c r="AC17" s="17">
+      <c r="AB17" s="14">
+        <v>6</v>
+      </c>
+      <c r="AC17" s="14">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="12">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16" t="s">
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16" t="s">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16" t="s">
+      <c r="I18" s="13"/>
+      <c r="J18" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16" t="s">
+      <c r="K18" s="13"/>
+      <c r="L18" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16" t="s">
+      <c r="M18" s="13"/>
+      <c r="N18" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="17">
+      <c r="O18" s="13"/>
+      <c r="P18" s="14">
         <v>23</v>
       </c>
-      <c r="Q18" s="16" t="s">
+      <c r="Q18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="16" t="s">
+      <c r="R18" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="S18" s="16" t="s">
+      <c r="S18" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="T18" s="17">
-        <v>6</v>
-      </c>
-      <c r="U18" s="17">
-        <v>5</v>
-      </c>
-      <c r="V18" s="17">
+      <c r="T18" s="14">
+        <v>6</v>
+      </c>
+      <c r="U18" s="14">
+        <v>5</v>
+      </c>
+      <c r="V18" s="14">
         <v>1</v>
       </c>
-      <c r="W18" s="17">
+      <c r="W18" s="14">
         <v>7</v>
       </c>
-      <c r="X18" s="17">
-        <v>5</v>
-      </c>
-      <c r="Y18" s="17">
-        <v>4</v>
-      </c>
-      <c r="Z18" s="17">
-        <v>6</v>
-      </c>
-      <c r="AA18" s="17">
-        <v>6</v>
-      </c>
-      <c r="AB18" s="17">
+      <c r="X18" s="14">
+        <v>5</v>
+      </c>
+      <c r="Y18" s="14">
+        <v>4</v>
+      </c>
+      <c r="Z18" s="14">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="14">
+        <v>6</v>
+      </c>
+      <c r="AB18" s="14">
         <v>3</v>
       </c>
-      <c r="AC18" s="17">
+      <c r="AC18" s="14">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
-      <c r="A19" s="12">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18" t="s">
+      <c r="E19" s="15"/>
+      <c r="F19" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18" t="s">
+      <c r="G19" s="15"/>
+      <c r="H19" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18" t="s">
+      <c r="I19" s="15"/>
+      <c r="J19" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18" t="s">
+      <c r="K19" s="15"/>
+      <c r="L19" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18" t="s">
+      <c r="M19" s="15"/>
+      <c r="N19" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="O19" s="18"/>
-      <c r="P19" s="19">
+      <c r="O19" s="15"/>
+      <c r="P19" s="16">
         <v>23</v>
       </c>
-      <c r="Q19" s="18" t="s">
+      <c r="Q19" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R19" s="16" t="s">
+      <c r="R19" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="S19" s="18" t="s">
+      <c r="S19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="T19" s="19">
+      <c r="T19" s="16">
         <v>2</v>
       </c>
-      <c r="U19" s="19">
+      <c r="U19" s="16">
         <v>2</v>
       </c>
-      <c r="V19" s="19">
-        <v>5</v>
-      </c>
-      <c r="W19" s="19">
-        <v>6</v>
-      </c>
-      <c r="X19" s="19">
-        <v>4</v>
-      </c>
-      <c r="Y19" s="19">
+      <c r="V19" s="16">
+        <v>5</v>
+      </c>
+      <c r="W19" s="16">
+        <v>6</v>
+      </c>
+      <c r="X19" s="16">
+        <v>4</v>
+      </c>
+      <c r="Y19" s="16">
         <v>7</v>
       </c>
-      <c r="Z19" s="19">
-        <v>6</v>
-      </c>
-      <c r="AA19" s="19">
-        <v>6</v>
-      </c>
-      <c r="AB19" s="19">
+      <c r="Z19" s="16">
+        <v>6</v>
+      </c>
+      <c r="AA19" s="16">
+        <v>6</v>
+      </c>
+      <c r="AB19" s="16">
         <v>2</v>
       </c>
-      <c r="AC19" s="19">
+      <c r="AC19" s="16">
         <v>4</v>
       </c>
     </row>
@@ -2987,53 +2978,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="7" width="20.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -3180,13 +3171,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="5">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>45366.237233796295</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="2">
         <v>45366.24219907408</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -3223,7 +3214,7 @@
         <v>55</v>
       </c>
       <c r="S2" s="3"/>
-      <c r="T2" s="5">
+      <c r="T2" s="1">
         <v>24</v>
       </c>
       <c r="U2" s="3" t="s">
@@ -3250,46 +3241,46 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="3"/>
-      <c r="AK2" s="5">
+      <c r="AK2" s="1">
         <v>2</v>
       </c>
-      <c r="AL2" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM2" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN2" s="5">
+      <c r="AL2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN2" s="1">
         <v>2</v>
       </c>
-      <c r="AO2" s="5">
-        <v>6</v>
-      </c>
-      <c r="AP2" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ2" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR2" s="5">
+      <c r="AO2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR2" s="1">
         <v>2</v>
       </c>
-      <c r="AS2" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT2" s="5">
+      <c r="AS2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT2" s="1">
         <v>4</v>
       </c>
       <c r="AU2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="5">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
         <v>45369.665555555555</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="2">
         <v>45369.674409722225</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3330,7 +3321,7 @@
         <v>69</v>
       </c>
       <c r="S3" s="3"/>
-      <c r="T3" s="5">
+      <c r="T3" s="1">
         <v>23</v>
       </c>
       <c r="U3" s="3" t="s">
@@ -3357,46 +3348,46 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="3"/>
-      <c r="AK3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AL3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AM3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN3" s="5">
+      <c r="AK3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN3" s="1">
         <v>7</v>
       </c>
-      <c r="AO3" s="5">
+      <c r="AO3" s="1">
         <v>2</v>
       </c>
-      <c r="AP3" s="5">
+      <c r="AP3" s="1">
         <v>2</v>
       </c>
-      <c r="AQ3" s="5">
+      <c r="AQ3" s="1">
         <v>7</v>
       </c>
-      <c r="AR3" s="5">
+      <c r="AR3" s="1">
         <v>1</v>
       </c>
-      <c r="AS3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT3" s="5">
+      <c r="AS3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT3" s="1">
         <v>4</v>
       </c>
       <c r="AU3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="5">
+      <c r="A4" s="1">
         <v>7</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>45369.67445601852</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="2">
         <v>45369.677939814814</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -3431,7 +3422,7 @@
         <v>76</v>
       </c>
       <c r="S4" s="3"/>
-      <c r="T4" s="5">
+      <c r="T4" s="1">
         <v>24</v>
       </c>
       <c r="U4" s="3" t="s">
@@ -3458,46 +3449,46 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="3"/>
-      <c r="AK4" s="5">
+      <c r="AK4" s="1">
         <v>2</v>
       </c>
-      <c r="AL4" s="5">
+      <c r="AL4" s="1">
         <v>3</v>
       </c>
-      <c r="AM4" s="5">
+      <c r="AM4" s="1">
         <v>2</v>
       </c>
-      <c r="AN4" s="5">
+      <c r="AN4" s="1">
         <v>2</v>
       </c>
-      <c r="AO4" s="5">
-        <v>4</v>
-      </c>
-      <c r="AP4" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ4" s="5">
-        <v>4</v>
-      </c>
-      <c r="AR4" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS4" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT4" s="5">
+      <c r="AO4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT4" s="1">
         <v>4</v>
       </c>
       <c r="AU4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="5">
+      <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>45369.680555555555</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="2">
         <v>45369.692337962966</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -3532,7 +3523,7 @@
         <v>84</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="T5" s="5">
+      <c r="T5" s="1">
         <v>27</v>
       </c>
       <c r="U5" s="3" t="s">
@@ -3559,46 +3550,46 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="3"/>
-      <c r="AK5" s="5">
-        <v>6</v>
-      </c>
-      <c r="AL5" s="5">
+      <c r="AK5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL5" s="1">
         <v>2</v>
       </c>
-      <c r="AM5" s="5">
-        <v>4</v>
-      </c>
-      <c r="AN5" s="5">
+      <c r="AM5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN5" s="1">
         <v>1</v>
       </c>
-      <c r="AO5" s="5">
-        <v>4</v>
-      </c>
-      <c r="AP5" s="5">
+      <c r="AO5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP5" s="1">
         <v>3</v>
       </c>
-      <c r="AQ5" s="5">
-        <v>6</v>
-      </c>
-      <c r="AR5" s="5">
+      <c r="AQ5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR5" s="1">
         <v>3</v>
       </c>
-      <c r="AS5" s="5">
-        <v>4</v>
-      </c>
-      <c r="AT5" s="5">
+      <c r="AS5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT5" s="1">
         <v>2</v>
       </c>
       <c r="AU5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>45369.67796296296</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>45369.706342592595</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -3635,7 +3626,7 @@
       <c r="S6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="1">
         <v>24</v>
       </c>
       <c r="U6" s="3" t="s">
@@ -3662,46 +3653,46 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="3"/>
-      <c r="AK6" s="5">
-        <v>6</v>
-      </c>
-      <c r="AL6" s="5">
+      <c r="AK6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL6" s="1">
         <v>1</v>
       </c>
-      <c r="AM6" s="5">
-        <v>4</v>
-      </c>
-      <c r="AN6" s="5">
-        <v>6</v>
-      </c>
-      <c r="AO6" s="5">
-        <v>6</v>
-      </c>
-      <c r="AP6" s="5">
-        <v>6</v>
-      </c>
-      <c r="AQ6" s="5">
-        <v>6</v>
-      </c>
-      <c r="AR6" s="5">
+      <c r="AM6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR6" s="1">
         <v>1</v>
       </c>
-      <c r="AS6" s="5">
+      <c r="AS6" s="1">
         <v>2</v>
       </c>
-      <c r="AT6" s="5">
+      <c r="AT6" s="1">
         <v>3</v>
       </c>
       <c r="AU6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="5">
+      <c r="A7" s="1">
         <v>11</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>45369.74828703704</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="2">
         <v>45369.758888888886</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -3738,7 +3729,7 @@
       <c r="S7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="1">
         <v>24</v>
       </c>
       <c r="U7" s="3" t="s">
@@ -3765,46 +3756,46 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="5">
+      <c r="AK7" s="1">
         <v>3</v>
       </c>
-      <c r="AL7" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM7" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN7" s="5">
-        <v>4</v>
-      </c>
-      <c r="AO7" s="5">
-        <v>6</v>
-      </c>
-      <c r="AP7" s="5">
+      <c r="AL7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AP7" s="1">
         <v>7</v>
       </c>
-      <c r="AQ7" s="5">
+      <c r="AQ7" s="1">
         <v>7</v>
       </c>
-      <c r="AR7" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS7" s="5">
-        <v>6</v>
-      </c>
-      <c r="AT7" s="5">
+      <c r="AR7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AT7" s="1">
         <v>6</v>
       </c>
       <c r="AU7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="5">
+      <c r="A8" s="1">
         <v>13</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>45369.99180555555</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="2">
         <v>45370.00729166667</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -3841,7 +3832,7 @@
       <c r="S8" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="1">
         <v>28</v>
       </c>
       <c r="U8" s="3" t="s">
@@ -3868,46 +3859,46 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="3"/>
-      <c r="AK8" s="5">
-        <v>4</v>
-      </c>
-      <c r="AL8" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM8" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN8" s="5">
-        <v>4</v>
-      </c>
-      <c r="AO8" s="5">
-        <v>5</v>
-      </c>
-      <c r="AP8" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ8" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR8" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS8" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT8" s="5">
+      <c r="AK8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT8" s="1">
         <v>4</v>
       </c>
       <c r="AU8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="5">
+      <c r="A9" s="1">
         <v>14</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>45370.66559027778</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="2">
         <v>45370.671944444446</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -3954,7 +3945,7 @@
       <c r="S9" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="1">
         <v>21</v>
       </c>
       <c r="U9" s="3" t="s">
@@ -3983,46 +3974,46 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="5">
-        <v>4</v>
-      </c>
-      <c r="AL9" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM9" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN9" s="5">
-        <v>4</v>
-      </c>
-      <c r="AO9" s="5">
-        <v>5</v>
-      </c>
-      <c r="AP9" s="5">
-        <v>4</v>
-      </c>
-      <c r="AQ9" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR9" s="5">
-        <v>5</v>
-      </c>
-      <c r="AS9" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT9" s="5">
+      <c r="AK9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AS9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT9" s="1">
         <v>5</v>
       </c>
       <c r="AU9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="5">
+      <c r="A10" s="1">
         <v>16</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>45376.08630787037</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="2">
         <v>45376.09385416667</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -4059,7 +4050,7 @@
       <c r="S10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="1">
         <v>23</v>
       </c>
       <c r="U10" s="3" t="s">
@@ -4086,46 +4077,46 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="5">
+      <c r="AK10" s="1">
         <v>7</v>
       </c>
-      <c r="AL10" s="5">
+      <c r="AL10" s="1">
         <v>2</v>
       </c>
-      <c r="AM10" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN10" s="5">
+      <c r="AM10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN10" s="1">
         <v>3</v>
       </c>
-      <c r="AO10" s="5">
-        <v>6</v>
-      </c>
-      <c r="AP10" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ10" s="5">
-        <v>6</v>
-      </c>
-      <c r="AR10" s="5">
+      <c r="AO10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR10" s="1">
         <v>3</v>
       </c>
-      <c r="AS10" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT10" s="5">
+      <c r="AS10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT10" s="1">
         <v>3</v>
       </c>
       <c r="AU10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="5">
+      <c r="A11" s="1">
         <v>17</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="2">
         <v>45376.974652777775</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="2">
         <v>45376.98210648148</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -4160,7 +4151,7 @@
         <v>142</v>
       </c>
       <c r="S11" s="3"/>
-      <c r="T11" s="5">
+      <c r="T11" s="1">
         <v>24</v>
       </c>
       <c r="U11" s="3" t="s">
@@ -4187,46 +4178,46 @@
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="3"/>
-      <c r="AK11" s="5">
+      <c r="AK11" s="1">
         <v>3</v>
       </c>
-      <c r="AL11" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM11" s="5">
-        <v>4</v>
-      </c>
-      <c r="AN11" s="5">
-        <v>4</v>
-      </c>
-      <c r="AO11" s="5">
-        <v>4</v>
-      </c>
-      <c r="AP11" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ11" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR11" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS11" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT11" s="5">
+      <c r="AL11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT11" s="1">
         <v>5</v>
       </c>
       <c r="AU11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="5">
+      <c r="A12" s="1">
         <v>20</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="2">
         <v>45376.99010416667</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="2">
         <v>45376.99548611111</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -4263,7 +4254,7 @@
       <c r="S12" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T12" s="1">
         <v>24</v>
       </c>
       <c r="U12" s="3" t="s">
@@ -4290,46 +4281,46 @@
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="3"/>
-      <c r="AK12" s="5">
+      <c r="AK12" s="1">
         <v>7</v>
       </c>
-      <c r="AL12" s="5">
-        <v>6</v>
-      </c>
-      <c r="AM12" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN12" s="5">
+      <c r="AL12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN12" s="1">
         <v>3</v>
       </c>
-      <c r="AO12" s="5">
+      <c r="AO12" s="1">
         <v>7</v>
       </c>
-      <c r="AP12" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ12" s="5">
-        <v>6</v>
-      </c>
-      <c r="AR12" s="5">
+      <c r="AP12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR12" s="1">
         <v>3</v>
       </c>
-      <c r="AS12" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT12" s="5">
+      <c r="AS12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT12" s="1">
         <v>3</v>
       </c>
       <c r="AU12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="5">
+      <c r="A13" s="1">
         <v>22</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="2">
         <v>45376.9955787037</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="2">
         <v>45377.004537037035</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -4368,7 +4359,7 @@
       <c r="S13" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="T13" s="5">
+      <c r="T13" s="1">
         <v>24</v>
       </c>
       <c r="U13" s="3" t="s">
@@ -4395,46 +4386,46 @@
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
       <c r="AJ13" s="3"/>
-      <c r="AK13" s="5">
+      <c r="AK13" s="1">
         <v>1</v>
       </c>
-      <c r="AL13" s="5">
+      <c r="AL13" s="1">
         <v>1</v>
       </c>
-      <c r="AM13" s="5">
-        <v>4</v>
-      </c>
-      <c r="AN13" s="5">
-        <v>4</v>
-      </c>
-      <c r="AO13" s="5">
-        <v>4</v>
-      </c>
-      <c r="AP13" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ13" s="5">
-        <v>4</v>
-      </c>
-      <c r="AR13" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS13" s="5">
-        <v>4</v>
-      </c>
-      <c r="AT13" s="5">
+      <c r="AM13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT13" s="1">
         <v>6</v>
       </c>
       <c r="AU13" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="5">
+      <c r="A14" s="1">
         <v>23</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="2">
         <v>45376.99458333333</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="2">
         <v>45377.00487268518</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -4469,7 +4460,7 @@
         <v>159</v>
       </c>
       <c r="S14" s="3"/>
-      <c r="T14" s="5">
+      <c r="T14" s="1">
         <v>24</v>
       </c>
       <c r="U14" s="3" t="s">
@@ -4496,46 +4487,46 @@
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
       <c r="AJ14" s="3"/>
-      <c r="AK14" s="5">
+      <c r="AK14" s="1">
         <v>3</v>
       </c>
-      <c r="AL14" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN14" s="5">
-        <v>4</v>
-      </c>
-      <c r="AO14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AP14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR14" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS14" s="5">
-        <v>4</v>
-      </c>
-      <c r="AT14" s="5">
+      <c r="AL14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO14" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP14" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ14" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT14" s="1">
         <v>2</v>
       </c>
       <c r="AU14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="5">
+      <c r="A15" s="1">
         <v>25</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="2">
         <v>45377.010567129626</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="2">
         <v>45377.02153935185</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -4570,7 +4561,7 @@
         <v>165</v>
       </c>
       <c r="S15" s="3"/>
-      <c r="T15" s="5">
+      <c r="T15" s="1">
         <v>27</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -4599,46 +4590,46 @@
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
       <c r="AJ15" s="3"/>
-      <c r="AK15" s="5">
+      <c r="AK15" s="1">
         <v>3</v>
       </c>
-      <c r="AL15" s="5">
+      <c r="AL15" s="1">
         <v>3</v>
       </c>
-      <c r="AM15" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN15" s="5">
+      <c r="AM15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN15" s="1">
         <v>3</v>
       </c>
-      <c r="AO15" s="5">
+      <c r="AO15" s="1">
         <v>3</v>
       </c>
-      <c r="AP15" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ15" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR15" s="5">
+      <c r="AP15" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ15" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR15" s="1">
         <v>1</v>
       </c>
-      <c r="AS15" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT15" s="5">
+      <c r="AS15" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT15" s="1">
         <v>4</v>
       </c>
       <c r="AU15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="5">
+      <c r="A16" s="1">
         <v>26</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="2">
         <v>45377.01954861111</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="2">
         <v>45377.025625</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -4675,7 +4666,7 @@
       <c r="S16" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="T16" s="5">
+      <c r="T16" s="1">
         <v>24</v>
       </c>
       <c r="U16" s="3" t="s">
@@ -4704,46 +4695,46 @@
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="3"/>
-      <c r="AK16" s="5">
-        <v>6</v>
-      </c>
-      <c r="AL16" s="5">
+      <c r="AK16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL16" s="1">
         <v>2</v>
       </c>
-      <c r="AM16" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN16" s="5">
-        <v>5</v>
-      </c>
-      <c r="AO16" s="5">
+      <c r="AM16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AO16" s="1">
         <v>1</v>
       </c>
-      <c r="AP16" s="5">
-        <v>4</v>
-      </c>
-      <c r="AQ16" s="5">
+      <c r="AP16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ16" s="1">
         <v>3</v>
       </c>
-      <c r="AR16" s="5">
+      <c r="AR16" s="1">
         <v>1</v>
       </c>
-      <c r="AS16" s="5">
-        <v>4</v>
-      </c>
-      <c r="AT16" s="5">
+      <c r="AS16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT16" s="1">
         <v>5</v>
       </c>
       <c r="AU16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="5">
+      <c r="A17" s="1">
         <v>29</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="2">
         <v>45377.05107638889</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="2">
         <v>45377.056122685186</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -4780,7 +4771,7 @@
       <c r="S17" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="T17" s="5">
+      <c r="T17" s="1">
         <v>23</v>
       </c>
       <c r="U17" s="3" t="s">
@@ -4807,46 +4798,46 @@
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
       <c r="AJ17" s="3"/>
-      <c r="AK17" s="5">
-        <v>6</v>
-      </c>
-      <c r="AL17" s="5">
-        <v>4</v>
-      </c>
-      <c r="AM17" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN17" s="5">
-        <v>6</v>
-      </c>
-      <c r="AO17" s="5">
+      <c r="AK17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AO17" s="1">
         <v>7</v>
       </c>
-      <c r="AP17" s="5">
+      <c r="AP17" s="1">
         <v>7</v>
       </c>
-      <c r="AQ17" s="5">
+      <c r="AQ17" s="1">
         <v>7</v>
       </c>
-      <c r="AR17" s="5">
+      <c r="AR17" s="1">
         <v>3</v>
       </c>
-      <c r="AS17" s="5">
+      <c r="AS17" s="1">
         <v>7</v>
       </c>
-      <c r="AT17" s="5">
+      <c r="AT17" s="1">
         <v>2</v>
       </c>
       <c r="AU17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="5">
+      <c r="A18" s="1">
         <v>30</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="2">
         <v>45377.08751157407</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="2">
         <v>45377.0955787037</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -4883,7 +4874,7 @@
       <c r="S18" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="1">
         <v>23</v>
       </c>
       <c r="U18" s="3" t="s">
@@ -4912,46 +4903,46 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
       <c r="AJ18" s="3"/>
-      <c r="AK18" s="5">
-        <v>4</v>
-      </c>
-      <c r="AL18" s="5">
-        <v>6</v>
-      </c>
-      <c r="AM18" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN18" s="5">
-        <v>5</v>
-      </c>
-      <c r="AO18" s="5">
+      <c r="AK18" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN18" s="1">
+        <v>5</v>
+      </c>
+      <c r="AO18" s="1">
         <v>7</v>
       </c>
-      <c r="AP18" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ18" s="5">
+      <c r="AP18" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ18" s="1">
         <v>7</v>
       </c>
-      <c r="AR18" s="5">
+      <c r="AR18" s="1">
         <v>1</v>
       </c>
-      <c r="AS18" s="5">
-        <v>6</v>
-      </c>
-      <c r="AT18" s="5">
+      <c r="AS18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AT18" s="1">
         <v>4</v>
       </c>
       <c r="AU18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="5">
+      <c r="A19" s="1">
         <v>32</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="2">
         <v>45377.40304398148</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="2">
         <v>45377.41028935185</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -4988,7 +4979,7 @@
       <c r="S19" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="T19" s="5">
+      <c r="T19" s="1">
         <v>28</v>
       </c>
       <c r="U19" s="3" t="s">
@@ -5017,46 +5008,46 @@
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
       <c r="AJ19" s="3"/>
-      <c r="AK19" s="5">
-        <v>4</v>
-      </c>
-      <c r="AL19" s="5">
+      <c r="AK19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL19" s="1">
         <v>1</v>
       </c>
-      <c r="AM19" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN19" s="5">
+      <c r="AM19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN19" s="1">
         <v>2</v>
       </c>
-      <c r="AO19" s="5">
-        <v>4</v>
-      </c>
-      <c r="AP19" s="5">
-        <v>6</v>
-      </c>
-      <c r="AQ19" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR19" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS19" s="5">
-        <v>4</v>
-      </c>
-      <c r="AT19" s="5">
+      <c r="AO19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT19" s="1">
         <v>3</v>
       </c>
       <c r="AU19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="5">
+      <c r="A20" s="1">
         <v>33</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="2">
         <v>45377.4005787037</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="2">
         <v>45377.41621527778</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -5093,7 +5084,7 @@
       <c r="S20" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="1">
         <v>23</v>
       </c>
       <c r="U20" s="3" t="s">
@@ -5111,77 +5102,77 @@
       <c r="Y20" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="Z20" s="5">
-        <v>5</v>
-      </c>
-      <c r="AA20" s="5">
+      <c r="Z20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA20" s="1">
         <v>2</v>
       </c>
-      <c r="AB20" s="5">
-        <v>6</v>
-      </c>
-      <c r="AC20" s="5">
+      <c r="AB20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="1">
         <v>7</v>
       </c>
-      <c r="AD20" s="5">
-        <v>5</v>
-      </c>
-      <c r="AE20" s="5">
-        <v>4</v>
-      </c>
-      <c r="AF20" s="5">
+      <c r="AD20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="1">
         <v>7</v>
       </c>
-      <c r="AG20" s="5">
+      <c r="AG20" s="1">
         <v>2</v>
       </c>
-      <c r="AH20" s="5">
-        <v>5</v>
-      </c>
-      <c r="AI20" s="5">
+      <c r="AH20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI20" s="1">
         <v>2</v>
       </c>
       <c r="AJ20" s="3"/>
-      <c r="AK20" s="5">
-        <v>5</v>
-      </c>
-      <c r="AL20" s="5">
+      <c r="AK20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL20" s="1">
         <v>2</v>
       </c>
-      <c r="AM20" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN20" s="5">
+      <c r="AM20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN20" s="1">
         <v>7</v>
       </c>
-      <c r="AO20" s="5">
-        <v>5</v>
-      </c>
-      <c r="AP20" s="5">
-        <v>4</v>
-      </c>
-      <c r="AQ20" s="5">
+      <c r="AO20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ20" s="1">
         <v>7</v>
       </c>
-      <c r="AR20" s="5">
+      <c r="AR20" s="1">
         <v>2</v>
       </c>
-      <c r="AS20" s="5">
-        <v>5</v>
-      </c>
-      <c r="AT20" s="5">
+      <c r="AS20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT20" s="1">
         <v>2</v>
       </c>
       <c r="AU20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="5">
+      <c r="A21" s="1">
         <v>35</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="2">
         <v>45377.977430555555</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="2">
         <v>45377.98799768519</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -5222,7 +5213,7 @@
         <v>214</v>
       </c>
       <c r="S21" s="3"/>
-      <c r="T21" s="5">
+      <c r="T21" s="1">
         <v>25</v>
       </c>
       <c r="U21" s="3" t="s">
@@ -5251,34 +5242,34 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="3"/>
-      <c r="AK21" s="5">
+      <c r="AK21" s="1">
         <v>3</v>
       </c>
-      <c r="AL21" s="5">
-        <v>5</v>
-      </c>
-      <c r="AM21" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN21" s="5">
+      <c r="AL21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN21" s="1">
         <v>2</v>
       </c>
-      <c r="AO21" s="5">
-        <v>6</v>
-      </c>
-      <c r="AP21" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ21" s="5">
-        <v>6</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>5</v>
-      </c>
-      <c r="AS21" s="5">
-        <v>6</v>
-      </c>
-      <c r="AT21" s="5">
+      <c r="AO21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AP21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AS21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AT21" s="1">
         <v>3</v>
       </c>
       <c r="AU21" s="3"/>

</xml_diff>